<commit_message>
corrected file endings in Excel files
</commit_message>
<xml_diff>
--- a/data/additional/primary/neptune/tsv/metadata_neptune.xlsx
+++ b/data/additional/primary/neptune/tsv/metadata_neptune.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luw52cg\Desktop\metadata_primary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub_RW\corpus\data\additional\primary\neptune\tsv\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0452139B-249A-4721-A1A3-D1BE4380F181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="6840" yWindow="2310" windowWidth="24660" windowHeight="14400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,24 +64,6 @@
     <t>quotes</t>
   </si>
   <si>
-    <t>rwk1_digbib_300-1.xmi</t>
-  </si>
-  <si>
-    <t>rwk1_digbib_1039-1.xmi</t>
-  </si>
-  <si>
-    <t>rwk1_digbib_1057-1.xmi</t>
-  </si>
-  <si>
-    <t>rwk1_mkhz_2778-1.xmi</t>
-  </si>
-  <si>
-    <t>rwk1_mkhz_6147-1.xmi</t>
-  </si>
-  <si>
-    <t>rwk1_mkhz_6263-1.xmi</t>
-  </si>
-  <si>
     <t>neptune</t>
   </si>
   <si>
@@ -196,12 +179,30 @@
   </si>
   <si>
     <t>german</t>
+  </si>
+  <si>
+    <t>rwk1_digbib_300-1.tsv</t>
+  </si>
+  <si>
+    <t>rwk1_digbib_1039-1.tsv</t>
+  </si>
+  <si>
+    <t>rwk1_digbib_1057-1.tsv</t>
+  </si>
+  <si>
+    <t>rwk1_mkhz_2778-1.tsv</t>
+  </si>
+  <si>
+    <t>rwk1_mkhz_6147-1.tsv</t>
+  </si>
+  <si>
+    <t>rwk1_mkhz_6263-1.tsv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -352,6 +353,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -387,6 +405,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -562,11 +597,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:U1048576"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,266 +652,266 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
       <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" t="s">
-        <v>27</v>
-      </c>
       <c r="E2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="H2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="I2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M2" t="s">
         <v>47</v>
       </c>
-      <c r="J2" t="s">
-        <v>49</v>
-      </c>
-      <c r="K2" t="s">
-        <v>47</v>
-      </c>
-      <c r="L2" t="s">
-        <v>48</v>
-      </c>
-      <c r="M2" t="s">
-        <v>53</v>
-      </c>
       <c r="N2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
         <v>22</v>
       </c>
-      <c r="D3" t="s">
-        <v>28</v>
-      </c>
       <c r="E3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" t="s">
         <v>41</v>
       </c>
-      <c r="H3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I3" t="s">
-        <v>47</v>
-      </c>
       <c r="J3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="K3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="L3" t="s">
+        <v>42</v>
+      </c>
+      <c r="M3" t="s">
         <v>48</v>
       </c>
-      <c r="M3" t="s">
-        <v>54</v>
-      </c>
       <c r="N3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
         <v>23</v>
       </c>
-      <c r="D4" t="s">
-        <v>29</v>
-      </c>
       <c r="E4" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F4" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="H4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="I4" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="J4" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="K4" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="L4" t="s">
+        <v>42</v>
+      </c>
+      <c r="M4" t="s">
         <v>48</v>
       </c>
-      <c r="M4" t="s">
-        <v>54</v>
-      </c>
       <c r="N4" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
         <v>24</v>
       </c>
-      <c r="D5" t="s">
-        <v>30</v>
-      </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G5" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="H5" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="I5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" t="s">
+        <v>42</v>
+      </c>
+      <c r="L5" t="s">
+        <v>42</v>
+      </c>
+      <c r="M5" t="s">
         <v>48</v>
       </c>
-      <c r="J5" t="s">
-        <v>50</v>
-      </c>
-      <c r="K5" t="s">
-        <v>48</v>
-      </c>
-      <c r="L5" t="s">
-        <v>48</v>
-      </c>
-      <c r="M5" t="s">
-        <v>54</v>
-      </c>
       <c r="N5" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
         <v>25</v>
       </c>
-      <c r="D6" t="s">
-        <v>31</v>
-      </c>
       <c r="E6" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="G6" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="H6" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="I6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" t="s">
+        <v>42</v>
+      </c>
+      <c r="L6" t="s">
+        <v>42</v>
+      </c>
+      <c r="M6" t="s">
         <v>48</v>
       </c>
-      <c r="J6" t="s">
-        <v>51</v>
-      </c>
-      <c r="K6" t="s">
-        <v>48</v>
-      </c>
-      <c r="L6" t="s">
-        <v>48</v>
-      </c>
-      <c r="M6" t="s">
-        <v>54</v>
-      </c>
       <c r="N6" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
         <v>20</v>
       </c>
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F7" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="G7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="H7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="I7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="J7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K7" t="s">
+        <v>42</v>
+      </c>
+      <c r="L7" t="s">
+        <v>42</v>
+      </c>
+      <c r="M7" t="s">
+        <v>49</v>
+      </c>
+      <c r="N7" t="s">
         <v>52</v>
-      </c>
-      <c r="K7" t="s">
-        <v>48</v>
-      </c>
-      <c r="L7" t="s">
-        <v>48</v>
-      </c>
-      <c r="M7" t="s">
-        <v>55</v>
-      </c>
-      <c r="N7" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>